<commit_message>
Updated - marked red weird stuff on results file
</commit_message>
<xml_diff>
--- a/analysis/25-07-2018 - tmp - table4michal.xlsx
+++ b/analysis/25-07-2018 - tmp - table4michal.xlsx
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -70,13 +70,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,16 +101,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -396,7 +413,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -467,7 +484,7 @@
       <c r="G2" s="2">
         <v>2.7678048780487798</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
         <v>0.982949260042284</v>
       </c>
       <c r="I2" s="1">
@@ -499,7 +516,7 @@
       <c r="G3" s="2">
         <v>2.7678048780487798</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="4">
         <v>0.982949260042284</v>
       </c>
       <c r="I3" s="1">
@@ -531,7 +548,7 @@
       <c r="G4" s="2">
         <v>3.2097560975609798</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="4">
         <v>1</v>
       </c>
       <c r="I4" s="1">
@@ -563,7 +580,7 @@
       <c r="G5" s="2">
         <v>3.2097560975609798</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="4">
         <v>1</v>
       </c>
       <c r="I5" s="1">
@@ -595,7 +612,7 @@
       <c r="G6" s="2">
         <v>4.8174358974359004</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>0.96420051167252496</v>
       </c>
       <c r="I6" s="1">
@@ -627,7 +644,7 @@
       <c r="G7" s="2">
         <v>4.8174358974359004</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>0.96420051167252496</v>
       </c>
       <c r="I7" s="1">
@@ -659,7 +676,7 @@
       <c r="G8" s="2">
         <v>5.7717948717948699</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>0.97181483850336203</v>
       </c>
       <c r="I8" s="1">
@@ -691,7 +708,7 @@
       <c r="G9" s="2">
         <v>5.7717948717948699</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>0.97181483850336203</v>
       </c>
       <c r="I9" s="1">
@@ -711,10 +728,10 @@
       <c r="C10">
         <v>0.1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>1934.0239999999999</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>1889.77966480447</v>
       </c>
       <c r="F10" s="2">
@@ -723,7 +740,7 @@
       <c r="G10" s="2">
         <v>18.046033519553099</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>0.58971711456860199</v>
       </c>
       <c r="I10" s="1">
@@ -743,10 +760,10 @@
       <c r="C11">
         <v>0.2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>2078.0479999999998</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>1889.77966480447</v>
       </c>
       <c r="F11" s="2">
@@ -755,7 +772,7 @@
       <c r="G11" s="2">
         <v>18.046033519553099</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>0.58971711456860199</v>
       </c>
       <c r="I11" s="1">
@@ -787,7 +804,7 @@
       <c r="G12" s="2">
         <v>20.057541899441301</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="4">
         <v>0.83674681753889801</v>
       </c>
       <c r="I12" s="1">
@@ -819,7 +836,7 @@
       <c r="G13" s="2">
         <v>20.057541899441301</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <v>0.83674681753889801</v>
       </c>
       <c r="I13" s="1">
@@ -851,7 +868,7 @@
       <c r="G14" s="2">
         <v>32.885476772616101</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <v>0.59620626739653604</v>
       </c>
       <c r="I14" s="1">
@@ -883,7 +900,7 @@
       <c r="G15" s="2">
         <v>32.885476772616101</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>0.59620626739653604</v>
       </c>
       <c r="I15" s="1">
@@ -915,7 +932,7 @@
       <c r="G16" s="2">
         <v>38.606845965770198</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>0.74785416643786895</v>
       </c>
       <c r="I16" s="1">
@@ -947,7 +964,7 @@
       <c r="G17" s="2">
         <v>38.606845965770198</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <v>0.74785416643786895</v>
       </c>
       <c r="I17" s="1">

</xml_diff>